<commit_message>
sofia test 1 added
</commit_message>
<xml_diff>
--- a/assets/fleet/9245263_sofia/datasets/Loads/SSS_Sofia_CargoData.xlsx
+++ b/assets/fleet/9245263_sofia/datasets/Loads/SSS_Sofia_CargoData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MERENKOV\Desktop\Капитан\sss\assets\fleet\9245263_sofia\datasets\Loads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF67C5B1-9DD3-4261-A2FA-3BC6FCAC62AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2730D3B3-4FD0-473E-8096-C58634A3B634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="797" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="797" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Soafia_GrainBulkheads" sheetId="24" r:id="rId1"/>
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2458" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2466" uniqueCount="155">
   <si>
     <t>Code</t>
   </si>
@@ -573,6 +573,12 @@
   </si>
   <si>
     <t>H104</t>
+  </si>
+  <si>
+    <t>SP102</t>
+  </si>
+  <si>
+    <t>SP202</t>
   </si>
 </sst>
 </file>
@@ -1089,10 +1095,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1107,11 +1113,11 @@
     <col min="8" max="8" width="9.28515625" style="5" customWidth="1"/>
     <col min="9" max="9" width="8.85546875" style="12"/>
     <col min="10" max="10" width="8.85546875" style="1"/>
-    <col min="11" max="13" width="8.85546875" style="5"/>
-    <col min="14" max="16384" width="8.85546875" style="4"/>
+    <col min="11" max="12" width="8.85546875" style="5"/>
+    <col min="13" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
@@ -1144,9 +1150,8 @@
       </c>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>8</v>
       </c>
@@ -1166,10 +1171,11 @@
         <v>73.358000000000004</v>
       </c>
       <c r="G2" s="14">
-        <v>75.988</v>
+        <v>74.673000000000002</v>
       </c>
       <c r="H2" s="14">
-        <v>74.673000000000002</v>
+        <f>(G2+F2)/2</f>
+        <v>74.015500000000003</v>
       </c>
       <c r="I2" s="14">
         <v>0</v>
@@ -1179,64 +1185,66 @@
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="21">
-        <v>105.18</v>
-      </c>
-      <c r="G3" s="21">
-        <v>105.92</v>
-      </c>
-      <c r="H3" s="22">
-        <v>105.5</v>
-      </c>
-      <c r="I3" s="10">
+        <v>153</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="9">
+        <v>1001</v>
+      </c>
+      <c r="F3" s="14">
+        <v>74.673000000000002</v>
+      </c>
+      <c r="G3" s="14">
+        <v>75.988</v>
+      </c>
+      <c r="H3" s="14">
+        <f>(G3+F3)/2</f>
+        <v>75.330500000000001</v>
+      </c>
+      <c r="I3" s="14">
         <v>0</v>
       </c>
-      <c r="J3" s="11">
-        <v>6.5019999999999998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J3" s="15">
+        <v>6.53</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="E4" s="9">
-        <v>1001</v>
+        <v>64</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="F4" s="21">
-        <v>96.3</v>
+        <v>105.18</v>
       </c>
       <c r="G4" s="21">
-        <v>97.04</v>
+        <v>105.92</v>
       </c>
       <c r="H4" s="22">
-        <v>96.882999999999996</v>
+        <v>105.5</v>
       </c>
       <c r="I4" s="10">
         <v>0</v>
@@ -1245,30 +1253,30 @@
         <v>6.5019999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="14">
-        <v>92.6</v>
-      </c>
-      <c r="G5" s="14">
-        <v>93.34</v>
+        <v>65</v>
+      </c>
+      <c r="E5" s="9">
+        <v>1001</v>
+      </c>
+      <c r="F5" s="21">
+        <v>96.3</v>
+      </c>
+      <c r="G5" s="21">
+        <v>97.04</v>
       </c>
       <c r="H5" s="22">
-        <v>92.92</v>
+        <v>96.882999999999996</v>
       </c>
       <c r="I5" s="10">
         <v>0</v>
@@ -1276,133 +1284,135 @@
       <c r="J5" s="11">
         <v>6.5019999999999998</v>
       </c>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" s="9">
-        <v>1002</v>
+        <v>42</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="F6" s="14">
-        <v>18.600000000000001</v>
+        <v>92.6</v>
       </c>
       <c r="G6" s="14">
-        <v>21.23</v>
-      </c>
-      <c r="H6" s="10">
-        <v>19.913</v>
+        <v>93.34</v>
+      </c>
+      <c r="H6" s="22">
+        <v>92.92</v>
       </c>
       <c r="I6" s="10">
         <v>0</v>
       </c>
-      <c r="J6" s="15">
-        <v>6.53</v>
+      <c r="J6" s="11">
+        <v>6.5019999999999998</v>
       </c>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="21">
-        <v>57.82</v>
-      </c>
-      <c r="G7" s="21">
-        <v>58.56</v>
-      </c>
-      <c r="H7" s="22">
-        <v>58.084000000000003</v>
+        <v>49</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="9">
+        <v>1002</v>
+      </c>
+      <c r="F7" s="14">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="G7" s="10">
+        <v>19.913</v>
+      </c>
+      <c r="H7" s="14">
+        <f>(G7+F7)/2</f>
+        <v>19.256500000000003</v>
       </c>
       <c r="I7" s="10">
         <v>0</v>
       </c>
-      <c r="J7" s="11">
-        <v>6.5019999999999998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J7" s="15">
+        <v>6.53</v>
+      </c>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>68</v>
+        <v>154</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>54</v>
       </c>
       <c r="E8" s="9">
         <v>1002</v>
       </c>
-      <c r="F8" s="21">
-        <v>54.12</v>
-      </c>
-      <c r="G8" s="21">
-        <v>54.86</v>
-      </c>
-      <c r="H8" s="22">
-        <v>54.276000000000003</v>
+      <c r="F8" s="10">
+        <v>19.913</v>
+      </c>
+      <c r="G8" s="14">
+        <v>21.23</v>
+      </c>
+      <c r="H8" s="14">
+        <f>(G8+F8)/2</f>
+        <v>20.5715</v>
       </c>
       <c r="I8" s="10">
         <v>0</v>
       </c>
-      <c r="J8" s="11">
-        <v>6.5019999999999998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J8" s="15">
+        <v>6.53</v>
+      </c>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>33</v>
       </c>
       <c r="F9" s="21">
-        <v>41.54</v>
+        <v>57.82</v>
       </c>
       <c r="G9" s="21">
-        <v>42.28</v>
+        <v>58.56</v>
       </c>
       <c r="H9" s="22">
-        <v>41.86</v>
+        <v>58.084000000000003</v>
       </c>
       <c r="I9" s="10">
         <v>0</v>
@@ -1411,30 +1421,30 @@
         <v>6.5019999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E10" s="9">
         <v>1002</v>
       </c>
       <c r="F10" s="21">
-        <v>31.18</v>
+        <v>54.12</v>
       </c>
       <c r="G10" s="21">
-        <v>31.92</v>
+        <v>54.86</v>
       </c>
       <c r="H10" s="22">
-        <v>31.5</v>
+        <v>54.276000000000003</v>
       </c>
       <c r="I10" s="10">
         <v>0</v>
@@ -1443,30 +1453,30 @@
         <v>6.5019999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>33</v>
       </c>
       <c r="F11" s="21">
-        <v>25.26</v>
+        <v>41.54</v>
       </c>
       <c r="G11" s="21">
-        <v>26</v>
+        <v>42.28</v>
       </c>
       <c r="H11" s="22">
-        <v>25.58</v>
+        <v>41.86</v>
       </c>
       <c r="I11" s="10">
         <v>0</v>
@@ -1475,10 +1485,74 @@
         <v>6.5019999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="9">
+        <v>1002</v>
+      </c>
+      <c r="F12" s="21">
+        <v>31.18</v>
+      </c>
+      <c r="G12" s="21">
+        <v>31.92</v>
+      </c>
+      <c r="H12" s="22">
+        <v>31.5</v>
+      </c>
+      <c r="I12" s="10">
+        <v>0</v>
+      </c>
+      <c r="J12" s="11">
+        <v>6.5019999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="21">
+        <v>25.26</v>
+      </c>
+      <c r="G13" s="21">
+        <v>26</v>
+      </c>
+      <c r="H13" s="22">
+        <v>25.58</v>
+      </c>
+      <c r="I13" s="10">
+        <v>0</v>
+      </c>
+      <c r="J13" s="11">
+        <v>6.5019999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -1596,8 +1670,8 @@
   </sheetPr>
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
sofia | bug fix
</commit_message>
<xml_diff>
--- a/assets/fleet/9245263_sofia/datasets/Loads/SSS_Sofia_CargoData.xlsx
+++ b/assets/fleet/9245263_sofia/datasets/Loads/SSS_Sofia_CargoData.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MERENKOV\Desktop\Капитан\sss\assets\fleet\9245263_sofia\datasets\Loads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA9ED8D0-47A2-4D24-B793-00D775FEDB1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE60432-5368-4162-8CA0-483531424D1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="797" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="797" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Soafia_GrainBulkheads" sheetId="24" r:id="rId1"/>
-    <sheet name="Soafia_GrainBulkheadsPlace" sheetId="26" r:id="rId2"/>
-    <sheet name="Soafia_CargoCompartments" sheetId="27" r:id="rId3"/>
-    <sheet name="Soafia_CargoCompartmentsParts" sheetId="28" r:id="rId4"/>
-    <sheet name="Soafia_сontainer_deck_plan" sheetId="29" r:id="rId5"/>
+    <sheet name="GrainBulkheads" sheetId="24" r:id="rId1"/>
+    <sheet name="GrainBulkheadsPlace" sheetId="26" r:id="rId2"/>
+    <sheet name="CargoCompartments" sheetId="27" r:id="rId3"/>
+    <sheet name="CargoCompartmentsParts" sheetId="28" r:id="rId4"/>
+    <sheet name="сontainer_deck_plan" sheetId="29" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -921,8 +921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2120,7 +2120,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Q235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+    <sheetView topLeftCell="A148" workbookViewId="0">
       <selection activeCell="F213" sqref="F213:F214"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
sofia | cargodata | fix
</commit_message>
<xml_diff>
--- a/assets/fleet/9245263_sofia/datasets/Loads/SSS_Sofia_CargoData.xlsx
+++ b/assets/fleet/9245263_sofia/datasets/Loads/SSS_Sofia_CargoData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MERENKOV\Desktop\Капитан\sss\assets\fleet\9245263_sofia\datasets\Loads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EDA6018-E751-4990-AEFC-D05E1EED7347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C3763B8-E0C7-4349-9DCA-77A026C8E4DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GrainBulkheads" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="CargoCompartmentsParts" sheetId="4" r:id="rId4"/>
     <sheet name="сontainer_deck_plan" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -98,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="128">
   <si>
     <t>Name  RUS</t>
   </si>
@@ -332,9 +332,6 @@
   </si>
   <si>
     <t>H104</t>
-  </si>
-  <si>
-    <t>103</t>
   </si>
   <si>
     <t>1104</t>
@@ -1463,7 +1460,7 @@
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L25" sqref="L24:L25"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1670,7 +1667,7 @@
         <v>77</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="H7" s="19">
         <v>92.6</v>
@@ -1684,7 +1681,7 @@
         <v>52</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>77</v>
@@ -1693,7 +1690,7 @@
         <v>24</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>63</v>
@@ -1713,10 +1710,10 @@
         <v>52</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>38</v>
@@ -1742,7 +1739,7 @@
         <v>52</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>35</v>
@@ -1754,10 +1751,10 @@
         <v>65</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H10" s="19">
         <v>57.82</v>
@@ -1771,10 +1768,10 @@
         <v>52</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>38</v>
@@ -1800,7 +1797,7 @@
         <v>52</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>39</v>
@@ -1812,10 +1809,10 @@
         <v>71</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H12" s="19">
         <v>54.12</v>
@@ -1829,10 +1826,10 @@
         <v>52</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>38</v>
@@ -1858,7 +1855,7 @@
         <v>52</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>42</v>
@@ -1870,10 +1867,10 @@
         <v>76</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H14" s="19">
         <v>41.54</v>
@@ -1887,16 +1884,16 @@
         <v>52</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>45</v>
@@ -1916,7 +1913,7 @@
         <v>52</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>45</v>
@@ -1925,13 +1922,13 @@
         <v>38</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="G16" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H16" s="19">
         <v>31.18</v>
@@ -1945,16 +1942,16 @@
         <v>52</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>48</v>
@@ -1974,7 +1971,7 @@
         <v>52</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>48</v>
@@ -1983,13 +1980,13 @@
         <v>38</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="G18" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H18" s="19">
         <v>25.26</v>
@@ -2003,16 +2000,16 @@
         <v>52</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>63</v>
@@ -2166,34 +2163,34 @@
   <sheetData>
     <row r="1" spans="1:17" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="C1" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="D1" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="E1" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="F1" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="G1" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="H1" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="I1" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="J1" s="24" t="s">
         <v>110</v>
-      </c>
-      <c r="J1" s="24" t="s">
-        <v>111</v>
       </c>
       <c r="N1" s="27"/>
       <c r="O1" s="24"/>
@@ -2205,7 +2202,7 @@
         <v>62</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C2" s="24" t="s">
         <v>65</v>
@@ -2313,7 +2310,7 @@
         <v>65</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C5" s="24" t="s">
         <v>65</v>
@@ -2417,7 +2414,7 @@
         <v>69</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C8" s="24" t="s">
         <v>65</v>
@@ -2577,7 +2574,7 @@
         <v>74</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C13" s="24" t="s">
         <v>65</v>
@@ -2737,7 +2734,7 @@
         <v>76</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C18" s="24" t="s">
         <v>65</v>
@@ -2894,10 +2891,10 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C23" s="24" t="s">
         <v>65</v>
@@ -2926,7 +2923,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B24" s="24" t="s">
         <v>62</v>
@@ -2958,7 +2955,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B25" s="24" t="s">
         <v>65</v>
@@ -2990,7 +2987,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B26" s="24" t="s">
         <v>69</v>
@@ -3022,7 +3019,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B27" s="24" t="s">
         <v>71</v>
@@ -3054,10 +3051,10 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B28" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C28" s="24" t="s">
         <v>65</v>
@@ -3086,7 +3083,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B29" s="24" t="s">
         <v>62</v>
@@ -3118,7 +3115,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B30" s="24" t="s">
         <v>65</v>
@@ -3150,7 +3147,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B31" s="24" t="s">
         <v>69</v>
@@ -3182,7 +3179,7 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B32" s="24" t="s">
         <v>71</v>
@@ -3214,10 +3211,10 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C33" s="24" t="s">
         <v>65</v>
@@ -3246,7 +3243,7 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B34" s="24" t="s">
         <v>62</v>
@@ -3278,7 +3275,7 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B35" s="24" t="s">
         <v>65</v>
@@ -3310,7 +3307,7 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B36" s="24" t="s">
         <v>69</v>
@@ -3342,7 +3339,7 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B37" s="24" t="s">
         <v>71</v>
@@ -3374,10 +3371,10 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B38" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C38" s="24" t="s">
         <v>65</v>
@@ -3406,7 +3403,7 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B39" s="24" t="s">
         <v>62</v>
@@ -3438,7 +3435,7 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B40" s="24" t="s">
         <v>65</v>
@@ -3470,7 +3467,7 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B41" s="24" t="s">
         <v>69</v>
@@ -3502,7 +3499,7 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B42" s="24" t="s">
         <v>71</v>
@@ -3534,10 +3531,10 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B43" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C43" s="24" t="s">
         <v>65</v>
@@ -3566,7 +3563,7 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B44" s="24" t="s">
         <v>62</v>
@@ -3598,7 +3595,7 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B45" s="24" t="s">
         <v>65</v>
@@ -3630,7 +3627,7 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B46" s="24" t="s">
         <v>69</v>
@@ -3662,7 +3659,7 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B47" s="24" t="s">
         <v>71</v>
@@ -3694,10 +3691,10 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B48" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C48" s="24" t="s">
         <v>65</v>
@@ -3726,7 +3723,7 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B49" s="24" t="s">
         <v>62</v>
@@ -3758,7 +3755,7 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B50" s="24" t="s">
         <v>65</v>
@@ -3790,7 +3787,7 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B51" s="24" t="s">
         <v>69</v>
@@ -3822,7 +3819,7 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B52" s="24" t="s">
         <v>71</v>
@@ -3854,10 +3851,10 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B53" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C53" s="24" t="s">
         <v>65</v>
@@ -3886,7 +3883,7 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B54" s="24" t="s">
         <v>62</v>
@@ -3918,7 +3915,7 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B55" s="24" t="s">
         <v>65</v>
@@ -3950,7 +3947,7 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B56" s="24" t="s">
         <v>69</v>
@@ -3982,7 +3979,7 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B57" s="24" t="s">
         <v>71</v>
@@ -4014,10 +4011,10 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B58" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C58" s="24" t="s">
         <v>65</v>
@@ -4046,7 +4043,7 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B59" s="24" t="s">
         <v>62</v>
@@ -4078,7 +4075,7 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B60" s="24" t="s">
         <v>65</v>
@@ -4110,7 +4107,7 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B61" s="24" t="s">
         <v>69</v>
@@ -4142,7 +4139,7 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B62" s="24" t="s">
         <v>71</v>
@@ -4174,10 +4171,10 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B63" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C63" s="24" t="s">
         <v>65</v>
@@ -4206,7 +4203,7 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B64" s="24" t="s">
         <v>62</v>
@@ -4238,7 +4235,7 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B65" s="24" t="s">
         <v>65</v>
@@ -4270,7 +4267,7 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B66" s="24" t="s">
         <v>69</v>
@@ -4302,7 +4299,7 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B67" s="24" t="s">
         <v>71</v>
@@ -4334,10 +4331,10 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B68" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C68" s="24" t="s">
         <v>65</v>
@@ -4366,7 +4363,7 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B69" s="24" t="s">
         <v>62</v>
@@ -4398,7 +4395,7 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B70" s="24" t="s">
         <v>65</v>
@@ -4430,7 +4427,7 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B71" s="24" t="s">
         <v>69</v>
@@ -4462,7 +4459,7 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B72" s="24" t="s">
         <v>71</v>
@@ -4494,10 +4491,10 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B73" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C73" s="24" t="s">
         <v>65</v>
@@ -4526,7 +4523,7 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B74" s="24" t="s">
         <v>62</v>
@@ -4558,7 +4555,7 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B75" s="24" t="s">
         <v>65</v>
@@ -4590,7 +4587,7 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B76" s="24" t="s">
         <v>69</v>
@@ -4622,7 +4619,7 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B77" s="24" t="s">
         <v>71</v>
@@ -4654,10 +4651,10 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B78" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C78" s="24" t="s">
         <v>65</v>
@@ -4686,7 +4683,7 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B79" s="24" t="s">
         <v>62</v>
@@ -4718,7 +4715,7 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B80" s="24" t="s">
         <v>65</v>
@@ -4750,7 +4747,7 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B81" s="24" t="s">
         <v>69</v>
@@ -4782,7 +4779,7 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B82" s="24" t="s">
         <v>71</v>
@@ -4814,10 +4811,10 @@
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B83" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C83" s="24" t="s">
         <v>65</v>
@@ -4846,7 +4843,7 @@
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B84" s="24" t="s">
         <v>62</v>
@@ -4878,7 +4875,7 @@
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B85" s="24" t="s">
         <v>65</v>
@@ -4910,7 +4907,7 @@
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B86" s="24" t="s">
         <v>69</v>
@@ -4942,7 +4939,7 @@
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B87" s="24" t="s">
         <v>71</v>
@@ -4974,10 +4971,10 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B88" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C88" s="24" t="s">
         <v>65</v>
@@ -5006,7 +5003,7 @@
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B89" s="24" t="s">
         <v>62</v>
@@ -5038,7 +5035,7 @@
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B90" s="24" t="s">
         <v>65</v>
@@ -5070,7 +5067,7 @@
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B91" s="24" t="s">
         <v>69</v>
@@ -5102,7 +5099,7 @@
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B92" s="24" t="s">
         <v>71</v>
@@ -5134,10 +5131,10 @@
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B93" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C93" s="24" t="s">
         <v>65</v>
@@ -5166,7 +5163,7 @@
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B94" s="24" t="s">
         <v>62</v>
@@ -5198,7 +5195,7 @@
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B95" s="24" t="s">
         <v>65</v>
@@ -5230,7 +5227,7 @@
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B96" s="24" t="s">
         <v>69</v>
@@ -5262,7 +5259,7 @@
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B97" s="24" t="s">
         <v>71</v>
@@ -5294,10 +5291,10 @@
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B98" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C98" s="24" t="s">
         <v>65</v>
@@ -5326,7 +5323,7 @@
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B99" s="24" t="s">
         <v>62</v>
@@ -5358,7 +5355,7 @@
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B100" s="24" t="s">
         <v>65</v>
@@ -5390,7 +5387,7 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B101" s="24" t="s">
         <v>69</v>
@@ -5422,7 +5419,7 @@
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B102" s="24" t="s">
         <v>71</v>
@@ -5454,10 +5451,10 @@
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B103" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C103" s="24" t="s">
         <v>65</v>
@@ -5486,7 +5483,7 @@
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B104" s="24" t="s">
         <v>62</v>
@@ -5518,7 +5515,7 @@
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B105" s="24" t="s">
         <v>65</v>
@@ -5550,7 +5547,7 @@
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B106" s="24" t="s">
         <v>69</v>
@@ -5582,7 +5579,7 @@
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B107" s="24" t="s">
         <v>71</v>
@@ -5617,10 +5614,10 @@
         <v>62</v>
       </c>
       <c r="B108" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C108" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D108" s="24" t="s">
         <v>65</v>
@@ -5652,7 +5649,7 @@
         <v>62</v>
       </c>
       <c r="C109" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D109" s="24" t="s">
         <v>65</v>
@@ -5684,7 +5681,7 @@
         <v>65</v>
       </c>
       <c r="C110" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D110" s="24" t="s">
         <v>65</v>
@@ -5716,7 +5713,7 @@
         <v>69</v>
       </c>
       <c r="C111" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D111" s="24" t="s">
         <v>65</v>
@@ -5748,7 +5745,7 @@
         <v>71</v>
       </c>
       <c r="C112" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D112" s="24" t="s">
         <v>65</v>
@@ -5777,10 +5774,10 @@
         <v>65</v>
       </c>
       <c r="B113" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C113" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D113" s="24" t="s">
         <v>71</v>
@@ -5812,7 +5809,7 @@
         <v>62</v>
       </c>
       <c r="C114" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D114" s="24" t="s">
         <v>71</v>
@@ -5844,7 +5841,7 @@
         <v>65</v>
       </c>
       <c r="C115" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D115" s="24" t="s">
         <v>71</v>
@@ -5876,7 +5873,7 @@
         <v>69</v>
       </c>
       <c r="C116" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D116" s="24" t="s">
         <v>71</v>
@@ -5908,7 +5905,7 @@
         <v>71</v>
       </c>
       <c r="C117" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D117" s="24" t="s">
         <v>71</v>
@@ -5937,10 +5934,10 @@
         <v>69</v>
       </c>
       <c r="B118" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C118" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D118" s="24" t="s">
         <v>65</v>
@@ -5972,7 +5969,7 @@
         <v>62</v>
       </c>
       <c r="C119" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D119" s="24" t="s">
         <v>65</v>
@@ -6004,7 +6001,7 @@
         <v>65</v>
       </c>
       <c r="C120" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D120" s="24" t="s">
         <v>65</v>
@@ -6036,7 +6033,7 @@
         <v>69</v>
       </c>
       <c r="C121" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D121" s="24" t="s">
         <v>65</v>
@@ -6068,7 +6065,7 @@
         <v>71</v>
       </c>
       <c r="C122" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D122" s="24" t="s">
         <v>65</v>
@@ -6097,10 +6094,10 @@
         <v>74</v>
       </c>
       <c r="B123" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C123" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D123" s="24" t="s">
         <v>65</v>
@@ -6132,7 +6129,7 @@
         <v>62</v>
       </c>
       <c r="C124" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D124" s="24" t="s">
         <v>65</v>
@@ -6164,7 +6161,7 @@
         <v>65</v>
       </c>
       <c r="C125" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D125" s="24" t="s">
         <v>65</v>
@@ -6196,7 +6193,7 @@
         <v>69</v>
       </c>
       <c r="C126" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D126" s="24" t="s">
         <v>65</v>
@@ -6228,7 +6225,7 @@
         <v>71</v>
       </c>
       <c r="C127" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D127" s="24" t="s">
         <v>65</v>
@@ -6257,10 +6254,10 @@
         <v>76</v>
       </c>
       <c r="B128" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C128" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D128" s="24" t="s">
         <v>71</v>
@@ -6292,7 +6289,7 @@
         <v>62</v>
       </c>
       <c r="C129" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D129" s="24" t="s">
         <v>71</v>
@@ -6324,7 +6321,7 @@
         <v>65</v>
       </c>
       <c r="C130" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D130" s="24" t="s">
         <v>71</v>
@@ -6356,7 +6353,7 @@
         <v>69</v>
       </c>
       <c r="C131" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D131" s="24" t="s">
         <v>71</v>
@@ -6382,13 +6379,13 @@
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B132" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C132" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D132" s="24" t="s">
         <v>65</v>
@@ -6414,13 +6411,13 @@
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B133" s="24" t="s">
         <v>62</v>
       </c>
       <c r="C133" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D133" s="24" t="s">
         <v>65</v>
@@ -6446,13 +6443,13 @@
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B134" s="24" t="s">
         <v>65</v>
       </c>
       <c r="C134" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D134" s="24" t="s">
         <v>65</v>
@@ -6478,13 +6475,13 @@
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B135" s="24" t="s">
         <v>69</v>
       </c>
       <c r="C135" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D135" s="24" t="s">
         <v>65</v>
@@ -6510,13 +6507,13 @@
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B136" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C136" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D136" s="24" t="s">
         <v>65</v>
@@ -6542,13 +6539,13 @@
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B137" s="24" t="s">
         <v>62</v>
       </c>
       <c r="C137" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D137" s="24" t="s">
         <v>65</v>
@@ -6574,13 +6571,13 @@
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B138" s="24" t="s">
         <v>65</v>
       </c>
       <c r="C138" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D138" s="24" t="s">
         <v>65</v>
@@ -6606,13 +6603,13 @@
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B139" s="24" t="s">
         <v>69</v>
       </c>
       <c r="C139" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D139" s="24" t="s">
         <v>65</v>
@@ -6638,13 +6635,13 @@
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B140" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C140" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D140" s="24" t="s">
         <v>65</v>
@@ -6670,13 +6667,13 @@
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B141" s="24" t="s">
         <v>62</v>
       </c>
       <c r="C141" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D141" s="24" t="s">
         <v>65</v>
@@ -6702,13 +6699,13 @@
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B142" s="24" t="s">
         <v>65</v>
       </c>
       <c r="C142" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D142" s="24" t="s">
         <v>65</v>
@@ -6734,13 +6731,13 @@
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B143" s="24" t="s">
         <v>69</v>
       </c>
       <c r="C143" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D143" s="24" t="s">
         <v>65</v>
@@ -6766,13 +6763,13 @@
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B144" s="24" t="s">
         <v>71</v>
       </c>
       <c r="C144" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D144" s="24" t="s">
         <v>65</v>
@@ -6798,13 +6795,13 @@
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B145" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C145" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D145" s="24" t="s">
         <v>71</v>
@@ -6830,13 +6827,13 @@
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B146" s="24" t="s">
         <v>62</v>
       </c>
       <c r="C146" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D146" s="24" t="s">
         <v>71</v>
@@ -6862,13 +6859,13 @@
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B147" s="24" t="s">
         <v>65</v>
       </c>
       <c r="C147" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D147" s="24" t="s">
         <v>71</v>
@@ -6894,13 +6891,13 @@
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B148" s="24" t="s">
         <v>69</v>
       </c>
       <c r="C148" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D148" s="24" t="s">
         <v>71</v>
@@ -6926,13 +6923,13 @@
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B149" s="24" t="s">
         <v>71</v>
       </c>
       <c r="C149" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D149" s="24" t="s">
         <v>71</v>
@@ -6958,13 +6955,13 @@
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B150" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C150" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D150" s="24" t="s">
         <v>65</v>
@@ -6990,13 +6987,13 @@
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B151" s="24" t="s">
         <v>62</v>
       </c>
       <c r="C151" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D151" s="24" t="s">
         <v>65</v>
@@ -7022,13 +7019,13 @@
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B152" s="24" t="s">
         <v>65</v>
       </c>
       <c r="C152" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D152" s="24" t="s">
         <v>65</v>
@@ -7054,13 +7051,13 @@
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B153" s="24" t="s">
         <v>69</v>
       </c>
       <c r="C153" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D153" s="24" t="s">
         <v>65</v>
@@ -7086,13 +7083,13 @@
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B154" s="24" t="s">
         <v>71</v>
       </c>
       <c r="C154" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D154" s="24" t="s">
         <v>65</v>
@@ -7118,13 +7115,13 @@
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B155" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C155" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D155" s="24" t="s">
         <v>65</v>
@@ -7150,13 +7147,13 @@
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B156" s="24" t="s">
         <v>62</v>
       </c>
       <c r="C156" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D156" s="24" t="s">
         <v>65</v>
@@ -7182,13 +7179,13 @@
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B157" s="24" t="s">
         <v>65</v>
       </c>
       <c r="C157" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D157" s="24" t="s">
         <v>65</v>
@@ -7214,13 +7211,13 @@
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B158" s="24" t="s">
         <v>69</v>
       </c>
       <c r="C158" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D158" s="24" t="s">
         <v>65</v>
@@ -7246,13 +7243,13 @@
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B159" s="24" t="s">
         <v>71</v>
       </c>
       <c r="C159" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D159" s="24" t="s">
         <v>65</v>
@@ -7278,13 +7275,13 @@
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B160" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C160" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D160" s="24" t="s">
         <v>71</v>
@@ -7310,13 +7307,13 @@
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B161" s="24" t="s">
         <v>62</v>
       </c>
       <c r="C161" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D161" s="24" t="s">
         <v>71</v>
@@ -7342,13 +7339,13 @@
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B162" s="24" t="s">
         <v>65</v>
       </c>
       <c r="C162" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D162" s="24" t="s">
         <v>71</v>
@@ -7374,13 +7371,13 @@
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B163" s="24" t="s">
         <v>69</v>
       </c>
       <c r="C163" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D163" s="24" t="s">
         <v>71</v>
@@ -7406,13 +7403,13 @@
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B164" s="24" t="s">
         <v>71</v>
       </c>
       <c r="C164" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D164" s="24" t="s">
         <v>71</v>
@@ -7438,13 +7435,13 @@
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B165" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C165" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D165" s="24" t="s">
         <v>65</v>
@@ -7470,13 +7467,13 @@
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B166" s="24" t="s">
         <v>62</v>
       </c>
       <c r="C166" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D166" s="24" t="s">
         <v>65</v>
@@ -7502,13 +7499,13 @@
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B167" s="24" t="s">
         <v>65</v>
       </c>
       <c r="C167" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D167" s="24" t="s">
         <v>65</v>
@@ -7534,13 +7531,13 @@
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B168" s="24" t="s">
         <v>69</v>
       </c>
       <c r="C168" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D168" s="24" t="s">
         <v>65</v>
@@ -7566,13 +7563,13 @@
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B169" s="24" t="s">
         <v>71</v>
       </c>
       <c r="C169" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D169" s="24" t="s">
         <v>65</v>
@@ -7598,13 +7595,13 @@
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B170" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C170" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D170" s="24" t="s">
         <v>65</v>
@@ -7630,13 +7627,13 @@
     </row>
     <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" s="24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B171" s="24" t="s">
         <v>62</v>
       </c>
       <c r="C171" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D171" s="24" t="s">
         <v>65</v>
@@ -7662,13 +7659,13 @@
     </row>
     <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B172" s="24" t="s">
         <v>65</v>
       </c>
       <c r="C172" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D172" s="24" t="s">
         <v>65</v>
@@ -7694,13 +7691,13 @@
     </row>
     <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B173" s="24" t="s">
         <v>69</v>
       </c>
       <c r="C173" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D173" s="24" t="s">
         <v>65</v>
@@ -7726,13 +7723,13 @@
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B174" s="24" t="s">
         <v>71</v>
       </c>
       <c r="C174" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D174" s="24" t="s">
         <v>65</v>
@@ -7758,13 +7755,13 @@
     </row>
     <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" s="24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B175" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C175" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D175" s="24" t="s">
         <v>71</v>
@@ -7790,13 +7787,13 @@
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B176" s="24" t="s">
         <v>62</v>
       </c>
       <c r="C176" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D176" s="24" t="s">
         <v>71</v>
@@ -7822,13 +7819,13 @@
     </row>
     <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B177" s="24" t="s">
         <v>65</v>
       </c>
       <c r="C177" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D177" s="24" t="s">
         <v>71</v>
@@ -7854,13 +7851,13 @@
     </row>
     <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B178" s="24" t="s">
         <v>69</v>
       </c>
       <c r="C178" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D178" s="24" t="s">
         <v>71</v>
@@ -7886,13 +7883,13 @@
     </row>
     <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B179" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C179" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D179" s="24" t="s">
         <v>65</v>
@@ -7918,13 +7915,13 @@
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B180" s="24" t="s">
         <v>62</v>
       </c>
       <c r="C180" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D180" s="24" t="s">
         <v>65</v>
@@ -7950,13 +7947,13 @@
     </row>
     <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B181" s="24" t="s">
         <v>65</v>
       </c>
       <c r="C181" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D181" s="24" t="s">
         <v>65</v>
@@ -7982,13 +7979,13 @@
     </row>
     <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B182" s="24" t="s">
         <v>69</v>
       </c>
       <c r="C182" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D182" s="24" t="s">
         <v>65</v>
@@ -8014,13 +8011,13 @@
     </row>
     <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B183" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C183" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D183" s="24" t="s">
         <v>65</v>
@@ -8046,13 +8043,13 @@
     </row>
     <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B184" s="24" t="s">
         <v>62</v>
       </c>
       <c r="C184" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D184" s="24" t="s">
         <v>65</v>
@@ -8078,13 +8075,13 @@
     </row>
     <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B185" s="24" t="s">
         <v>65</v>
       </c>
       <c r="C185" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D185" s="24" t="s">
         <v>65</v>
@@ -8110,13 +8107,13 @@
     </row>
     <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B186" s="24" t="s">
         <v>69</v>
       </c>
       <c r="C186" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D186" s="24" t="s">
         <v>65</v>
@@ -8142,13 +8139,13 @@
     </row>
     <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" s="24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B187" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C187" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D187" s="24" t="s">
         <v>71</v>
@@ -8174,13 +8171,13 @@
     </row>
     <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" s="24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B188" s="24" t="s">
         <v>62</v>
       </c>
       <c r="C188" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D188" s="24" t="s">
         <v>71</v>
@@ -8206,13 +8203,13 @@
     </row>
     <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" s="24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B189" s="24" t="s">
         <v>65</v>
       </c>
       <c r="C189" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D189" s="24" t="s">
         <v>71</v>
@@ -8238,13 +8235,13 @@
     </row>
     <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" s="24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B190" s="24" t="s">
         <v>69</v>
       </c>
       <c r="C190" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D190" s="24" t="s">
         <v>71</v>
@@ -8270,13 +8267,13 @@
     </row>
     <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" s="24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B191" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C191" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D191" s="24" t="s">
         <v>65</v>
@@ -8302,13 +8299,13 @@
     </row>
     <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" s="24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B192" s="24" t="s">
         <v>62</v>
       </c>
       <c r="C192" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D192" s="24" t="s">
         <v>65</v>
@@ -8334,13 +8331,13 @@
     </row>
     <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" s="24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B193" s="24" t="s">
         <v>65</v>
       </c>
       <c r="C193" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D193" s="24" t="s">
         <v>65</v>
@@ -8366,13 +8363,13 @@
     </row>
     <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" s="24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B194" s="24" t="s">
         <v>69</v>
       </c>
       <c r="C194" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D194" s="24" t="s">
         <v>65</v>
@@ -8398,13 +8395,13 @@
     </row>
     <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" s="24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B195" s="24" t="s">
         <v>71</v>
       </c>
       <c r="C195" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D195" s="24" t="s">
         <v>65</v>
@@ -8430,13 +8427,13 @@
     </row>
     <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" s="24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B196" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C196" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D196" s="24" t="s">
         <v>65</v>
@@ -8462,13 +8459,13 @@
     </row>
     <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" s="24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B197" s="24" t="s">
         <v>62</v>
       </c>
       <c r="C197" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D197" s="24" t="s">
         <v>65</v>
@@ -8494,13 +8491,13 @@
     </row>
     <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" s="24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B198" s="24" t="s">
         <v>65</v>
       </c>
       <c r="C198" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D198" s="24" t="s">
         <v>65</v>
@@ -8526,13 +8523,13 @@
     </row>
     <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" s="24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B199" s="24" t="s">
         <v>69</v>
       </c>
       <c r="C199" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D199" s="24" t="s">
         <v>65</v>
@@ -8558,13 +8555,13 @@
     </row>
     <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" s="24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B200" s="24" t="s">
         <v>71</v>
       </c>
       <c r="C200" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D200" s="24" t="s">
         <v>65</v>
@@ -8590,13 +8587,13 @@
     </row>
     <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" s="24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B201" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C201" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D201" s="24" t="s">
         <v>71</v>
@@ -8622,13 +8619,13 @@
     </row>
     <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202" s="24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B202" s="24" t="s">
         <v>62</v>
       </c>
       <c r="C202" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D202" s="24" t="s">
         <v>71</v>
@@ -8654,13 +8651,13 @@
     </row>
     <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" s="24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B203" s="24" t="s">
         <v>65</v>
       </c>
       <c r="C203" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D203" s="24" t="s">
         <v>71</v>
@@ -8686,13 +8683,13 @@
     </row>
     <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" s="24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B204" s="24" t="s">
         <v>69</v>
       </c>
       <c r="C204" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D204" s="24" t="s">
         <v>71</v>
@@ -8718,13 +8715,13 @@
     </row>
     <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205" s="24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B205" s="24" t="s">
         <v>71</v>
       </c>
       <c r="C205" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D205" s="24" t="s">
         <v>71</v>
@@ -8750,13 +8747,13 @@
     </row>
     <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B206" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C206" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D206" s="24" t="s">
         <v>65</v>
@@ -8782,13 +8779,13 @@
     </row>
     <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B207" s="24" t="s">
         <v>62</v>
       </c>
       <c r="C207" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D207" s="24" t="s">
         <v>65</v>
@@ -8814,13 +8811,13 @@
     </row>
     <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B208" s="24" t="s">
         <v>65</v>
       </c>
       <c r="C208" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D208" s="24" t="s">
         <v>65</v>
@@ -8846,13 +8843,13 @@
     </row>
     <row r="209" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A209" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B209" s="24" t="s">
         <v>69</v>
       </c>
       <c r="C209" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D209" s="24" t="s">
         <v>65</v>
@@ -8878,13 +8875,13 @@
     </row>
     <row r="210" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A210" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B210" s="24" t="s">
         <v>71</v>
       </c>
       <c r="C210" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D210" s="24" t="s">
         <v>65</v>
@@ -8910,13 +8907,13 @@
     </row>
     <row r="211" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A211" s="24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B211" s="24" t="s">
         <v>62</v>
       </c>
       <c r="C211" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D211" s="24" t="s">
         <v>65</v>
@@ -8942,13 +8939,13 @@
     </row>
     <row r="212" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A212" s="24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B212" s="24" t="s">
         <v>65</v>
       </c>
       <c r="C212" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D212" s="24" t="s">
         <v>65</v>
@@ -8974,13 +8971,13 @@
     </row>
     <row r="213" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A213" s="24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B213" s="24" t="s">
         <v>69</v>
       </c>
       <c r="C213" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D213" s="24" t="s">
         <v>65</v>
@@ -9006,13 +9003,13 @@
     </row>
     <row r="214" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A214" s="24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B214" s="24" t="s">
         <v>71</v>
       </c>
       <c r="C214" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D214" s="24" t="s">
         <v>65</v>
@@ -9038,10 +9035,10 @@
     </row>
     <row r="215" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A215" s="24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B215" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C215" s="24" t="s">
         <v>65</v>
@@ -9070,7 +9067,7 @@
     </row>
     <row r="216" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A216" s="24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B216" s="24" t="s">
         <v>62</v>
@@ -9102,7 +9099,7 @@
     </row>
     <row r="217" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A217" s="24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B217" s="24" t="s">
         <v>65</v>
@@ -9134,7 +9131,7 @@
     </row>
     <row r="218" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A218" s="24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B218" s="24" t="s">
         <v>69</v>
@@ -9166,7 +9163,7 @@
     </row>
     <row r="219" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A219" s="24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B219" s="24" t="s">
         <v>71</v>
@@ -9198,10 +9195,10 @@
     </row>
     <row r="220" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A220" s="24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B220" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C220" s="24" t="s">
         <v>65</v>
@@ -9230,7 +9227,7 @@
     </row>
     <row r="221" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A221" s="24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B221" s="24" t="s">
         <v>62</v>
@@ -9262,7 +9259,7 @@
     </row>
     <row r="222" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A222" s="24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B222" s="24" t="s">
         <v>65</v>
@@ -9294,7 +9291,7 @@
     </row>
     <row r="223" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A223" s="24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B223" s="24" t="s">
         <v>69</v>
@@ -9326,7 +9323,7 @@
     </row>
     <row r="224" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A224" s="24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B224" s="24" t="s">
         <v>71</v>
@@ -9358,13 +9355,13 @@
     </row>
     <row r="225" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A225" s="24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B225" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C225" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D225" s="24" t="s">
         <v>69</v>
@@ -9390,13 +9387,13 @@
     </row>
     <row r="226" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A226" s="24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B226" s="24" t="s">
         <v>62</v>
       </c>
       <c r="C226" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D226" s="24" t="s">
         <v>69</v>
@@ -9422,13 +9419,13 @@
     </row>
     <row r="227" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A227" s="24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B227" s="24" t="s">
         <v>65</v>
       </c>
       <c r="C227" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D227" s="24" t="s">
         <v>69</v>
@@ -9454,13 +9451,13 @@
     </row>
     <row r="228" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A228" s="24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B228" s="24" t="s">
         <v>69</v>
       </c>
       <c r="C228" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D228" s="24" t="s">
         <v>69</v>
@@ -9486,13 +9483,13 @@
     </row>
     <row r="229" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A229" s="24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B229" s="24" t="s">
         <v>71</v>
       </c>
       <c r="C229" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D229" s="24" t="s">
         <v>69</v>
@@ -9518,13 +9515,13 @@
     </row>
     <row r="230" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A230" s="24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B230" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C230" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D230" s="24" t="s">
         <v>69</v>
@@ -9550,13 +9547,13 @@
     </row>
     <row r="231" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A231" s="24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B231" s="24" t="s">
         <v>62</v>
       </c>
       <c r="C231" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D231" s="24" t="s">
         <v>69</v>
@@ -9582,13 +9579,13 @@
     </row>
     <row r="232" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A232" s="24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B232" s="24" t="s">
         <v>65</v>
       </c>
       <c r="C232" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D232" s="24" t="s">
         <v>69</v>
@@ -9614,13 +9611,13 @@
     </row>
     <row r="233" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A233" s="24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B233" s="24" t="s">
         <v>69</v>
       </c>
       <c r="C233" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D233" s="24" t="s">
         <v>69</v>
@@ -9646,13 +9643,13 @@
     </row>
     <row r="234" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A234" s="24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B234" s="24" t="s">
         <v>71</v>
       </c>
       <c r="C234" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D234" s="24" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
sofia | container fix
</commit_message>
<xml_diff>
--- a/assets/fleet/9245263_sofia/datasets/Loads/SSS_Sofia_CargoData.xlsx
+++ b/assets/fleet/9245263_sofia/datasets/Loads/SSS_Sofia_CargoData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MERENKOV\Desktop\Капитан\sss\assets\fleet\9245263_sofia\datasets\Loads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C3763B8-E0C7-4349-9DCA-77A026C8E4DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B85ECFA8-4322-46C0-8244-D34E8BAEBA9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GrainBulkheads" sheetId="1" r:id="rId1"/>
@@ -1459,7 +1459,7 @@
   </sheetPr>
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -2142,8 +2142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Q235"/>
   <sheetViews>
-    <sheetView topLeftCell="A148" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F213" sqref="F213"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2349,7 +2349,7 @@
         <v>62</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="D6" s="24" t="s">
         <v>71</v>
@@ -2385,7 +2385,7 @@
         <v>65</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="D7" s="24" t="s">
         <v>71</v>

</xml_diff>

<commit_message>
sofia | container | fix
</commit_message>
<xml_diff>
--- a/assets/fleet/9245263_sofia/datasets/Loads/SSS_Sofia_CargoData.xlsx
+++ b/assets/fleet/9245263_sofia/datasets/Loads/SSS_Sofia_CargoData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MERENKOV\Desktop\Капитан\sss\assets\fleet\9245263_sofia\datasets\Loads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B85ECFA8-4322-46C0-8244-D34E8BAEBA9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C9F811F-FD00-40E9-89AF-BCFF67289BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2143,7 +2143,7 @@
   <dimension ref="A1:Q235"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2222,10 +2222,10 @@
       <c r="H2" s="28">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I2" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J2" s="29">
+      <c r="I2" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J2" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="N2" s="27"/>
@@ -2258,10 +2258,10 @@
       <c r="H3" s="28">
         <v>3.72</v>
       </c>
-      <c r="I3" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J3" s="29">
+      <c r="I3" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J3" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="N3" s="27"/>
@@ -2294,10 +2294,10 @@
       <c r="H4" s="28">
         <v>3.72</v>
       </c>
-      <c r="I4" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J4" s="29">
+      <c r="I4" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J4" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="N4" s="27"/>
@@ -2330,10 +2330,10 @@
       <c r="H5" s="28">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I5" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J5" s="29">
+      <c r="I5" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J5" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="N5" s="27"/>
@@ -2364,12 +2364,12 @@
         <v>11.785</v>
       </c>
       <c r="H6" s="28">
-        <v>1.1160000000000001</v>
-      </c>
-      <c r="I6" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J6" s="29">
+        <v>3.72</v>
+      </c>
+      <c r="I6" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J6" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="N6" s="27"/>
@@ -2400,12 +2400,12 @@
         <v>11.785</v>
       </c>
       <c r="H7" s="28">
-        <v>1.1160000000000001</v>
-      </c>
-      <c r="I7" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J7" s="29">
+        <v>3.72</v>
+      </c>
+      <c r="I7" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J7" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -2434,10 +2434,10 @@
       <c r="H8" s="28">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I8" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J8" s="29">
+      <c r="I8" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J8" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -2466,10 +2466,10 @@
       <c r="H9" s="28">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I9" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J9" s="29">
+      <c r="I9" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J9" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -2498,10 +2498,10 @@
       <c r="H10" s="28">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I10" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J10" s="29">
+      <c r="I10" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J10" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -2530,10 +2530,10 @@
       <c r="H11" s="28">
         <v>6.3239999999999998</v>
       </c>
-      <c r="I11" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J11" s="29">
+      <c r="I11" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J11" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -2562,10 +2562,10 @@
       <c r="H12" s="28">
         <v>6.3239999999999998</v>
       </c>
-      <c r="I12" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J12" s="29">
+      <c r="I12" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J12" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -2594,10 +2594,10 @@
       <c r="H13" s="28">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I13" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J13" s="29">
+      <c r="I13" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J13" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -2626,10 +2626,10 @@
       <c r="H14" s="28">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I14" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J14" s="29">
+      <c r="I14" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J14" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -2658,10 +2658,10 @@
       <c r="H15" s="28">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I15" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J15" s="29">
+      <c r="I15" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J15" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -2690,10 +2690,10 @@
       <c r="H16" s="28">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I16" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J16" s="29">
+      <c r="I16" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J16" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -2722,10 +2722,10 @@
       <c r="H17" s="28">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I17" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J17" s="29">
+      <c r="I17" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J17" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -2754,10 +2754,10 @@
       <c r="H18" s="28">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I18" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J18" s="29">
+      <c r="I18" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J18" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -2786,10 +2786,10 @@
       <c r="H19" s="28">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I19" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J19" s="29">
+      <c r="I19" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J19" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -2818,10 +2818,10 @@
       <c r="H20" s="28">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I20" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J20" s="29">
+      <c r="I20" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J20" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -2850,10 +2850,10 @@
       <c r="H21" s="28">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I21" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J21" s="29">
+      <c r="I21" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J21" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -2882,10 +2882,10 @@
       <c r="H22" s="28">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I22" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J22" s="29">
+      <c r="I22" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J22" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -2914,10 +2914,10 @@
       <c r="H23" s="28">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I23" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J23" s="29">
+      <c r="I23" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J23" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -2946,10 +2946,10 @@
       <c r="H24" s="28">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I24" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J24" s="29">
+      <c r="I24" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J24" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -2978,10 +2978,10 @@
       <c r="H25" s="28">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I25" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J25" s="29">
+      <c r="I25" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J25" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -3010,10 +3010,10 @@
       <c r="H26" s="28">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I26" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J26" s="29">
+      <c r="I26" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J26" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -3042,10 +3042,10 @@
       <c r="H27" s="28">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I27" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J27" s="29">
+      <c r="I27" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J27" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -3074,10 +3074,10 @@
       <c r="H28" s="28">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I28" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J28" s="29">
+      <c r="I28" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J28" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -3106,10 +3106,10 @@
       <c r="H29" s="28">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I29" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J29" s="29">
+      <c r="I29" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J29" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -3138,10 +3138,10 @@
       <c r="H30" s="28">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I30" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J30" s="29">
+      <c r="I30" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J30" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -3170,10 +3170,10 @@
       <c r="H31" s="28">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I31" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J31" s="29">
+      <c r="I31" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J31" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -3202,10 +3202,10 @@
       <c r="H32" s="28">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I32" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J32" s="29">
+      <c r="I32" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J32" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -3234,10 +3234,10 @@
       <c r="H33" s="28">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I33" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J33" s="29">
+      <c r="I33" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J33" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -3266,10 +3266,10 @@
       <c r="H34" s="28">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I34" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J34" s="29">
+      <c r="I34" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J34" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -3298,10 +3298,10 @@
       <c r="H35" s="28">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I35" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J35" s="29">
+      <c r="I35" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J35" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -3330,10 +3330,10 @@
       <c r="H36" s="28">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I36" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J36" s="29">
+      <c r="I36" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J36" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -3362,10 +3362,10 @@
       <c r="H37" s="28">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I37" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J37" s="29">
+      <c r="I37" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J37" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -3394,10 +3394,10 @@
       <c r="H38" s="28">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I38" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J38" s="29">
+      <c r="I38" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J38" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -3426,10 +3426,10 @@
       <c r="H39" s="28">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I39" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J39" s="29">
+      <c r="I39" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J39" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -3458,10 +3458,10 @@
       <c r="H40" s="28">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I40" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J40" s="29">
+      <c r="I40" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J40" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -3490,10 +3490,10 @@
       <c r="H41" s="28">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I41" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J41" s="29">
+      <c r="I41" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J41" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -3522,10 +3522,10 @@
       <c r="H42" s="28">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I42" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J42" s="29">
+      <c r="I42" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J42" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -3554,10 +3554,10 @@
       <c r="H43" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I43" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J43" s="29">
+      <c r="I43" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J43" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -3586,10 +3586,10 @@
       <c r="H44" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I44" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J44" s="29">
+      <c r="I44" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J44" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -3618,10 +3618,10 @@
       <c r="H45" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I45" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J45" s="29">
+      <c r="I45" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J45" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -3650,10 +3650,10 @@
       <c r="H46" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I46" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J46" s="29">
+      <c r="I46" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J46" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -3682,10 +3682,10 @@
       <c r="H47" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I47" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J47" s="29">
+      <c r="I47" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J47" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -3714,10 +3714,10 @@
       <c r="H48" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I48" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J48" s="29">
+      <c r="I48" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J48" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -3746,10 +3746,10 @@
       <c r="H49" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I49" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J49" s="29">
+      <c r="I49" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J49" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -3778,10 +3778,10 @@
       <c r="H50" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I50" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J50" s="29">
+      <c r="I50" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J50" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -3810,10 +3810,10 @@
       <c r="H51" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I51" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J51" s="29">
+      <c r="I51" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J51" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -3842,10 +3842,10 @@
       <c r="H52" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I52" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J52" s="29">
+      <c r="I52" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J52" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -3874,10 +3874,10 @@
       <c r="H53" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I53" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J53" s="29">
+      <c r="I53" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J53" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -3906,10 +3906,10 @@
       <c r="H54" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I54" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J54" s="29">
+      <c r="I54" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J54" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -3938,10 +3938,10 @@
       <c r="H55" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I55" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J55" s="29">
+      <c r="I55" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J55" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -3970,10 +3970,10 @@
       <c r="H56" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I56" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J56" s="29">
+      <c r="I56" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J56" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -4002,10 +4002,10 @@
       <c r="H57" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I57" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J57" s="29">
+      <c r="I57" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J57" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -4034,10 +4034,10 @@
       <c r="H58" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I58" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J58" s="29">
+      <c r="I58" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J58" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -4066,10 +4066,10 @@
       <c r="H59" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I59" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J59" s="29">
+      <c r="I59" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J59" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -4098,10 +4098,10 @@
       <c r="H60" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I60" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J60" s="29">
+      <c r="I60" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J60" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -4130,10 +4130,10 @@
       <c r="H61" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I61" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J61" s="29">
+      <c r="I61" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J61" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -4162,10 +4162,10 @@
       <c r="H62" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I62" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J62" s="29">
+      <c r="I62" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J62" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -4194,10 +4194,10 @@
       <c r="H63" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I63" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J63" s="29">
+      <c r="I63" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J63" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -4226,10 +4226,10 @@
       <c r="H64" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I64" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J64" s="29">
+      <c r="I64" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J64" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -4258,10 +4258,10 @@
       <c r="H65" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I65" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J65" s="29">
+      <c r="I65" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J65" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -4290,10 +4290,10 @@
       <c r="H66" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I66" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J66" s="29">
+      <c r="I66" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J66" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -4322,10 +4322,10 @@
       <c r="H67" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I67" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J67" s="29">
+      <c r="I67" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J67" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -4354,10 +4354,10 @@
       <c r="H68" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I68" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J68" s="29">
+      <c r="I68" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J68" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -4386,10 +4386,10 @@
       <c r="H69" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I69" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J69" s="29">
+      <c r="I69" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J69" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -4418,10 +4418,10 @@
       <c r="H70" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I70" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J70" s="29">
+      <c r="I70" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J70" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -4450,10 +4450,10 @@
       <c r="H71" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I71" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J71" s="29">
+      <c r="I71" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J71" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -4482,10 +4482,10 @@
       <c r="H72" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I72" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J72" s="29">
+      <c r="I72" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J72" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -4514,10 +4514,10 @@
       <c r="H73" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I73" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J73" s="29">
+      <c r="I73" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J73" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -4546,10 +4546,10 @@
       <c r="H74" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I74" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J74" s="29">
+      <c r="I74" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J74" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -4578,10 +4578,10 @@
       <c r="H75" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I75" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J75" s="29">
+      <c r="I75" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J75" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -4610,10 +4610,10 @@
       <c r="H76" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I76" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J76" s="29">
+      <c r="I76" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J76" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -4642,10 +4642,10 @@
       <c r="H77" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I77" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J77" s="29">
+      <c r="I77" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J77" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -4674,10 +4674,10 @@
       <c r="H78" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I78" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J78" s="29">
+      <c r="I78" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J78" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -4706,10 +4706,10 @@
       <c r="H79" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I79" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J79" s="29">
+      <c r="I79" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J79" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -4738,10 +4738,10 @@
       <c r="H80" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I80" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J80" s="29">
+      <c r="I80" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J80" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -4770,10 +4770,10 @@
       <c r="H81" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I81" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J81" s="29">
+      <c r="I81" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J81" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -4802,10 +4802,10 @@
       <c r="H82" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I82" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J82" s="29">
+      <c r="I82" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J82" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -4834,10 +4834,10 @@
       <c r="H83" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I83" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J83" s="29">
+      <c r="I83" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J83" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -4866,10 +4866,10 @@
       <c r="H84" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I84" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J84" s="29">
+      <c r="I84" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J84" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -4898,10 +4898,10 @@
       <c r="H85" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I85" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J85" s="29">
+      <c r="I85" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J85" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -4930,10 +4930,10 @@
       <c r="H86" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I86" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J86" s="29">
+      <c r="I86" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J86" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -4962,10 +4962,10 @@
       <c r="H87" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I87" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J87" s="29">
+      <c r="I87" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J87" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -4994,10 +4994,10 @@
       <c r="H88" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I88" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J88" s="29">
+      <c r="I88" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J88" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -5026,10 +5026,10 @@
       <c r="H89" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I89" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J89" s="29">
+      <c r="I89" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J89" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -5058,10 +5058,10 @@
       <c r="H90" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I90" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J90" s="29">
+      <c r="I90" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J90" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -5090,10 +5090,10 @@
       <c r="H91" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I91" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J91" s="29">
+      <c r="I91" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J91" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -5122,10 +5122,10 @@
       <c r="H92" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I92" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J92" s="29">
+      <c r="I92" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J92" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -5154,10 +5154,10 @@
       <c r="H93" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I93" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J93" s="29">
+      <c r="I93" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J93" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -5186,10 +5186,10 @@
       <c r="H94" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I94" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J94" s="29">
+      <c r="I94" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J94" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -5218,10 +5218,10 @@
       <c r="H95" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I95" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J95" s="29">
+      <c r="I95" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J95" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -5250,10 +5250,10 @@
       <c r="H96" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I96" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J96" s="29">
+      <c r="I96" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J96" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -5282,10 +5282,10 @@
       <c r="H97" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I97" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J97" s="29">
+      <c r="I97" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J97" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -5314,10 +5314,10 @@
       <c r="H98" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I98" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J98" s="29">
+      <c r="I98" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J98" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -5346,10 +5346,10 @@
       <c r="H99" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I99" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J99" s="29">
+      <c r="I99" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J99" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -5378,10 +5378,10 @@
       <c r="H100" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I100" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J100" s="29">
+      <c r="I100" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J100" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -5410,10 +5410,10 @@
       <c r="H101" s="29">
         <v>3.72</v>
       </c>
-      <c r="I101" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J101" s="29">
+      <c r="I101" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J101" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -5442,10 +5442,10 @@
       <c r="H102" s="29">
         <v>3.72</v>
       </c>
-      <c r="I102" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J102" s="29">
+      <c r="I102" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J102" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -5474,10 +5474,10 @@
       <c r="H103" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I103" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J103" s="29">
+      <c r="I103" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J103" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -5506,10 +5506,10 @@
       <c r="H104" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I104" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J104" s="29">
+      <c r="I104" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J104" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -5538,10 +5538,10 @@
       <c r="H105" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I105" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J105" s="29">
+      <c r="I105" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J105" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -5570,10 +5570,10 @@
       <c r="H106" s="29">
         <v>3.72</v>
       </c>
-      <c r="I106" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J106" s="29">
+      <c r="I106" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J106" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -5602,10 +5602,10 @@
       <c r="H107" s="29">
         <v>3.72</v>
       </c>
-      <c r="I107" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J107" s="29">
+      <c r="I107" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J107" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -5634,10 +5634,10 @@
       <c r="H108" s="29">
         <v>12.536</v>
       </c>
-      <c r="I108" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J108" s="29">
+      <c r="I108" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J108" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -5666,10 +5666,10 @@
       <c r="H109" s="29">
         <v>12.536</v>
       </c>
-      <c r="I109" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J109" s="29">
+      <c r="I109" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J109" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -5698,10 +5698,10 @@
       <c r="H110" s="29">
         <v>12.536</v>
       </c>
-      <c r="I110" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J110" s="29">
+      <c r="I110" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J110" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -5730,10 +5730,10 @@
       <c r="H111" s="29">
         <v>12.536</v>
       </c>
-      <c r="I111" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J111" s="29">
+      <c r="I111" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J111" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -5762,10 +5762,10 @@
       <c r="H112" s="29">
         <v>12.536</v>
       </c>
-      <c r="I112" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J112" s="29">
+      <c r="I112" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J112" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -5794,10 +5794,10 @@
       <c r="H113" s="29">
         <v>12.536</v>
       </c>
-      <c r="I113" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J113" s="29">
+      <c r="I113" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J113" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -5826,10 +5826,10 @@
       <c r="H114" s="29">
         <v>12.536</v>
       </c>
-      <c r="I114" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J114" s="29">
+      <c r="I114" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J114" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -5858,10 +5858,10 @@
       <c r="H115" s="29">
         <v>12.536</v>
       </c>
-      <c r="I115" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J115" s="29">
+      <c r="I115" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J115" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -5890,10 +5890,10 @@
       <c r="H116" s="29">
         <v>12.536</v>
       </c>
-      <c r="I116" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J116" s="29">
+      <c r="I116" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J116" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -5922,10 +5922,10 @@
       <c r="H117" s="29">
         <v>12.536</v>
       </c>
-      <c r="I117" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J117" s="29">
+      <c r="I117" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J117" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -5954,10 +5954,10 @@
       <c r="H118" s="29">
         <v>12.536</v>
       </c>
-      <c r="I118" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J118" s="29">
+      <c r="I118" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J118" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -5986,10 +5986,10 @@
       <c r="H119" s="29">
         <v>12.536</v>
       </c>
-      <c r="I119" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J119" s="29">
+      <c r="I119" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J119" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -6018,10 +6018,10 @@
       <c r="H120" s="29">
         <v>12.536</v>
       </c>
-      <c r="I120" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J120" s="29">
+      <c r="I120" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J120" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -6050,10 +6050,10 @@
       <c r="H121" s="29">
         <v>12.536</v>
       </c>
-      <c r="I121" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J121" s="29">
+      <c r="I121" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J121" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -6082,10 +6082,10 @@
       <c r="H122" s="29">
         <v>12.536</v>
       </c>
-      <c r="I122" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J122" s="29">
+      <c r="I122" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J122" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -6114,10 +6114,10 @@
       <c r="H123" s="29">
         <v>12.536</v>
       </c>
-      <c r="I123" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J123" s="29">
+      <c r="I123" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J123" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -6146,10 +6146,10 @@
       <c r="H124" s="29">
         <v>12.536</v>
       </c>
-      <c r="I124" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J124" s="29">
+      <c r="I124" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J124" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -6178,10 +6178,10 @@
       <c r="H125" s="29">
         <v>12.536</v>
       </c>
-      <c r="I125" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J125" s="29">
+      <c r="I125" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J125" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -6210,10 +6210,10 @@
       <c r="H126" s="29">
         <v>12.536</v>
       </c>
-      <c r="I126" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J126" s="29">
+      <c r="I126" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J126" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -6242,10 +6242,10 @@
       <c r="H127" s="29">
         <v>12.536</v>
       </c>
-      <c r="I127" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J127" s="29">
+      <c r="I127" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J127" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -6274,10 +6274,10 @@
       <c r="H128" s="29">
         <v>12.536</v>
       </c>
-      <c r="I128" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J128" s="29">
+      <c r="I128" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J128" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -6306,10 +6306,10 @@
       <c r="H129" s="29">
         <v>12.536</v>
       </c>
-      <c r="I129" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J129" s="29">
+      <c r="I129" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J129" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -6338,10 +6338,10 @@
       <c r="H130" s="29">
         <v>12.536</v>
       </c>
-      <c r="I130" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J130" s="29">
+      <c r="I130" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J130" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -6370,10 +6370,10 @@
       <c r="H131" s="29">
         <v>12.536</v>
       </c>
-      <c r="I131" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J131" s="29">
+      <c r="I131" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J131" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -6402,10 +6402,10 @@
       <c r="H132" s="29">
         <v>12.536</v>
       </c>
-      <c r="I132" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J132" s="29">
+      <c r="I132" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J132" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -6434,10 +6434,10 @@
       <c r="H133" s="29">
         <v>12.536</v>
       </c>
-      <c r="I133" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J133" s="29">
+      <c r="I133" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J133" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -6466,10 +6466,10 @@
       <c r="H134" s="29">
         <v>12.536</v>
       </c>
-      <c r="I134" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J134" s="29">
+      <c r="I134" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J134" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -6498,10 +6498,10 @@
       <c r="H135" s="29">
         <v>12.536</v>
       </c>
-      <c r="I135" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J135" s="29">
+      <c r="I135" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J135" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -6530,10 +6530,10 @@
       <c r="H136" s="29">
         <v>12.536</v>
       </c>
-      <c r="I136" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J136" s="29">
+      <c r="I136" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J136" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -6562,10 +6562,10 @@
       <c r="H137" s="29">
         <v>12.536</v>
       </c>
-      <c r="I137" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J137" s="29">
+      <c r="I137" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J137" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -6594,10 +6594,10 @@
       <c r="H138" s="29">
         <v>12.536</v>
       </c>
-      <c r="I138" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J138" s="29">
+      <c r="I138" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J138" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -6626,10 +6626,10 @@
       <c r="H139" s="29">
         <v>12.536</v>
       </c>
-      <c r="I139" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J139" s="29">
+      <c r="I139" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J139" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -6658,10 +6658,10 @@
       <c r="H140" s="29">
         <v>12.536</v>
       </c>
-      <c r="I140" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J140" s="29">
+      <c r="I140" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J140" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -6690,10 +6690,10 @@
       <c r="H141" s="29">
         <v>12.536</v>
       </c>
-      <c r="I141" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J141" s="29">
+      <c r="I141" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J141" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -6722,10 +6722,10 @@
       <c r="H142" s="29">
         <v>12.536</v>
       </c>
-      <c r="I142" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J142" s="29">
+      <c r="I142" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J142" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -6754,10 +6754,10 @@
       <c r="H143" s="29">
         <v>12.536</v>
       </c>
-      <c r="I143" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J143" s="29">
+      <c r="I143" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J143" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -6786,10 +6786,10 @@
       <c r="H144" s="29">
         <v>12.536</v>
       </c>
-      <c r="I144" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J144" s="29">
+      <c r="I144" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J144" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -6818,10 +6818,10 @@
       <c r="H145" s="29">
         <v>12.536</v>
       </c>
-      <c r="I145" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J145" s="29">
+      <c r="I145" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J145" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -6850,10 +6850,10 @@
       <c r="H146" s="29">
         <v>12.536</v>
       </c>
-      <c r="I146" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J146" s="29">
+      <c r="I146" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J146" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -6882,10 +6882,10 @@
       <c r="H147" s="29">
         <v>12.536</v>
       </c>
-      <c r="I147" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J147" s="29">
+      <c r="I147" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J147" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -6914,10 +6914,10 @@
       <c r="H148" s="29">
         <v>12.536</v>
       </c>
-      <c r="I148" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J148" s="29">
+      <c r="I148" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J148" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -6946,10 +6946,10 @@
       <c r="H149" s="29">
         <v>12.536</v>
       </c>
-      <c r="I149" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J149" s="29">
+      <c r="I149" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J149" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -6978,10 +6978,10 @@
       <c r="H150" s="29">
         <v>12.536</v>
       </c>
-      <c r="I150" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J150" s="29">
+      <c r="I150" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J150" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -7010,10 +7010,10 @@
       <c r="H151" s="29">
         <v>12.536</v>
       </c>
-      <c r="I151" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J151" s="29">
+      <c r="I151" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J151" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -7042,10 +7042,10 @@
       <c r="H152" s="29">
         <v>12.536</v>
       </c>
-      <c r="I152" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J152" s="29">
+      <c r="I152" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J152" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -7074,10 +7074,10 @@
       <c r="H153" s="29">
         <v>12.536</v>
       </c>
-      <c r="I153" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J153" s="29">
+      <c r="I153" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J153" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -7106,10 +7106,10 @@
       <c r="H154" s="29">
         <v>12.536</v>
       </c>
-      <c r="I154" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J154" s="29">
+      <c r="I154" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J154" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -7138,10 +7138,10 @@
       <c r="H155" s="29">
         <v>12.536</v>
       </c>
-      <c r="I155" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J155" s="29">
+      <c r="I155" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J155" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -7170,10 +7170,10 @@
       <c r="H156" s="29">
         <v>12.536</v>
       </c>
-      <c r="I156" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J156" s="29">
+      <c r="I156" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J156" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -7202,10 +7202,10 @@
       <c r="H157" s="29">
         <v>12.536</v>
       </c>
-      <c r="I157" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J157" s="29">
+      <c r="I157" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J157" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -7234,10 +7234,10 @@
       <c r="H158" s="29">
         <v>12.536</v>
       </c>
-      <c r="I158" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J158" s="29">
+      <c r="I158" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J158" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -7266,10 +7266,10 @@
       <c r="H159" s="29">
         <v>12.536</v>
       </c>
-      <c r="I159" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J159" s="29">
+      <c r="I159" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J159" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -7298,10 +7298,10 @@
       <c r="H160" s="29">
         <v>12.536</v>
       </c>
-      <c r="I160" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J160" s="29">
+      <c r="I160" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J160" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -7330,10 +7330,10 @@
       <c r="H161" s="29">
         <v>12.536</v>
       </c>
-      <c r="I161" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J161" s="29">
+      <c r="I161" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J161" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -7362,10 +7362,10 @@
       <c r="H162" s="29">
         <v>12.536</v>
       </c>
-      <c r="I162" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J162" s="29">
+      <c r="I162" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J162" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -7394,10 +7394,10 @@
       <c r="H163" s="29">
         <v>12.536</v>
       </c>
-      <c r="I163" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J163" s="29">
+      <c r="I163" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J163" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -7426,10 +7426,10 @@
       <c r="H164" s="29">
         <v>12.536</v>
       </c>
-      <c r="I164" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J164" s="29">
+      <c r="I164" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J164" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -7458,10 +7458,10 @@
       <c r="H165" s="29">
         <v>12.536</v>
       </c>
-      <c r="I165" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J165" s="29">
+      <c r="I165" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J165" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -7490,10 +7490,10 @@
       <c r="H166" s="29">
         <v>12.536</v>
       </c>
-      <c r="I166" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J166" s="29">
+      <c r="I166" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J166" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -7522,10 +7522,10 @@
       <c r="H167" s="29">
         <v>12.536</v>
       </c>
-      <c r="I167" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J167" s="29">
+      <c r="I167" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J167" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -7554,10 +7554,10 @@
       <c r="H168" s="29">
         <v>12.536</v>
       </c>
-      <c r="I168" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J168" s="29">
+      <c r="I168" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J168" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -7586,10 +7586,10 @@
       <c r="H169" s="29">
         <v>12.536</v>
       </c>
-      <c r="I169" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J169" s="29">
+      <c r="I169" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J169" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -7618,10 +7618,10 @@
       <c r="H170" s="29">
         <v>12.536</v>
       </c>
-      <c r="I170" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J170" s="29">
+      <c r="I170" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J170" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -7650,10 +7650,10 @@
       <c r="H171" s="29">
         <v>12.536</v>
       </c>
-      <c r="I171" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J171" s="29">
+      <c r="I171" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J171" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -7682,10 +7682,10 @@
       <c r="H172" s="29">
         <v>12.536</v>
       </c>
-      <c r="I172" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J172" s="29">
+      <c r="I172" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J172" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -7714,10 +7714,10 @@
       <c r="H173" s="29">
         <v>12.536</v>
       </c>
-      <c r="I173" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J173" s="29">
+      <c r="I173" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J173" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -7746,10 +7746,10 @@
       <c r="H174" s="29">
         <v>12.536</v>
       </c>
-      <c r="I174" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J174" s="29">
+      <c r="I174" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J174" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -7778,10 +7778,10 @@
       <c r="H175" s="29">
         <v>12.536</v>
       </c>
-      <c r="I175" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J175" s="29">
+      <c r="I175" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J175" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -7810,10 +7810,10 @@
       <c r="H176" s="29">
         <v>12.536</v>
       </c>
-      <c r="I176" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J176" s="29">
+      <c r="I176" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J176" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -7842,10 +7842,10 @@
       <c r="H177" s="29">
         <v>12.536</v>
       </c>
-      <c r="I177" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J177" s="29">
+      <c r="I177" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J177" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -7874,10 +7874,10 @@
       <c r="H178" s="29">
         <v>12.536</v>
       </c>
-      <c r="I178" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J178" s="29">
+      <c r="I178" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J178" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -7906,10 +7906,10 @@
       <c r="H179" s="29">
         <v>12.536</v>
       </c>
-      <c r="I179" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J179" s="29">
+      <c r="I179" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J179" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -7938,10 +7938,10 @@
       <c r="H180" s="29">
         <v>12.536</v>
       </c>
-      <c r="I180" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J180" s="29">
+      <c r="I180" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J180" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -7970,10 +7970,10 @@
       <c r="H181" s="29">
         <v>12.536</v>
       </c>
-      <c r="I181" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J181" s="29">
+      <c r="I181" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J181" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -8002,10 +8002,10 @@
       <c r="H182" s="29">
         <v>12.536</v>
       </c>
-      <c r="I182" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J182" s="29">
+      <c r="I182" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J182" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -8034,10 +8034,10 @@
       <c r="H183" s="29">
         <v>12.536</v>
       </c>
-      <c r="I183" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J183" s="29">
+      <c r="I183" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J183" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -8066,10 +8066,10 @@
       <c r="H184" s="29">
         <v>12.536</v>
       </c>
-      <c r="I184" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J184" s="29">
+      <c r="I184" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J184" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -8098,10 +8098,10 @@
       <c r="H185" s="29">
         <v>12.536</v>
       </c>
-      <c r="I185" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J185" s="29">
+      <c r="I185" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J185" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -8130,10 +8130,10 @@
       <c r="H186" s="29">
         <v>12.536</v>
       </c>
-      <c r="I186" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J186" s="29">
+      <c r="I186" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J186" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -8162,10 +8162,10 @@
       <c r="H187" s="29">
         <v>12.536</v>
       </c>
-      <c r="I187" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J187" s="29">
+      <c r="I187" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J187" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -8194,10 +8194,10 @@
       <c r="H188" s="29">
         <v>12.536</v>
       </c>
-      <c r="I188" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J188" s="29">
+      <c r="I188" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J188" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -8226,10 +8226,10 @@
       <c r="H189" s="29">
         <v>12.536</v>
       </c>
-      <c r="I189" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J189" s="29">
+      <c r="I189" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J189" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -8258,10 +8258,10 @@
       <c r="H190" s="29">
         <v>12.536</v>
       </c>
-      <c r="I190" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J190" s="29">
+      <c r="I190" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J190" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -8290,10 +8290,10 @@
       <c r="H191" s="29">
         <v>12.536</v>
       </c>
-      <c r="I191" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J191" s="29">
+      <c r="I191" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J191" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -8322,10 +8322,10 @@
       <c r="H192" s="29">
         <v>12.536</v>
       </c>
-      <c r="I192" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J192" s="29">
+      <c r="I192" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J192" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -8354,10 +8354,10 @@
       <c r="H193" s="29">
         <v>12.536</v>
       </c>
-      <c r="I193" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J193" s="29">
+      <c r="I193" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J193" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -8386,10 +8386,10 @@
       <c r="H194" s="29">
         <v>12.536</v>
       </c>
-      <c r="I194" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J194" s="29">
+      <c r="I194" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J194" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -8418,10 +8418,10 @@
       <c r="H195" s="29">
         <v>12.536</v>
       </c>
-      <c r="I195" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J195" s="29">
+      <c r="I195" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J195" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -8450,10 +8450,10 @@
       <c r="H196" s="29">
         <v>12.536</v>
       </c>
-      <c r="I196" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J196" s="29">
+      <c r="I196" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J196" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -8482,10 +8482,10 @@
       <c r="H197" s="29">
         <v>12.536</v>
       </c>
-      <c r="I197" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J197" s="29">
+      <c r="I197" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J197" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -8514,10 +8514,10 @@
       <c r="H198" s="29">
         <v>12.536</v>
       </c>
-      <c r="I198" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J198" s="29">
+      <c r="I198" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J198" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -8546,10 +8546,10 @@
       <c r="H199" s="29">
         <v>12.536</v>
       </c>
-      <c r="I199" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J199" s="29">
+      <c r="I199" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J199" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -8578,10 +8578,10 @@
       <c r="H200" s="29">
         <v>12.536</v>
       </c>
-      <c r="I200" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J200" s="29">
+      <c r="I200" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J200" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -8610,10 +8610,10 @@
       <c r="H201" s="29">
         <v>12.536</v>
       </c>
-      <c r="I201" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J201" s="29">
+      <c r="I201" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J201" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -8642,10 +8642,10 @@
       <c r="H202" s="29">
         <v>12.536</v>
       </c>
-      <c r="I202" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J202" s="29">
+      <c r="I202" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J202" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -8674,10 +8674,10 @@
       <c r="H203" s="29">
         <v>12.536</v>
       </c>
-      <c r="I203" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J203" s="29">
+      <c r="I203" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J203" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -8706,10 +8706,10 @@
       <c r="H204" s="29">
         <v>12.536</v>
       </c>
-      <c r="I204" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J204" s="29">
+      <c r="I204" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J204" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -8738,10 +8738,10 @@
       <c r="H205" s="29">
         <v>12.536</v>
       </c>
-      <c r="I205" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J205" s="29">
+      <c r="I205" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J205" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -8770,10 +8770,10 @@
       <c r="H206" s="29">
         <v>12.536</v>
       </c>
-      <c r="I206" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J206" s="29">
+      <c r="I206" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J206" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -8802,10 +8802,10 @@
       <c r="H207" s="29">
         <v>12.536</v>
       </c>
-      <c r="I207" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J207" s="29">
+      <c r="I207" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J207" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -8834,10 +8834,10 @@
       <c r="H208" s="29">
         <v>12.536</v>
       </c>
-      <c r="I208" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J208" s="29">
+      <c r="I208" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J208" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -8866,10 +8866,10 @@
       <c r="H209" s="29">
         <v>12.536</v>
       </c>
-      <c r="I209" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J209" s="29">
+      <c r="I209" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J209" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -8898,10 +8898,10 @@
       <c r="H210" s="29">
         <v>12.536</v>
       </c>
-      <c r="I210" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J210" s="29">
+      <c r="I210" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J210" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -8930,10 +8930,10 @@
       <c r="H211" s="29">
         <v>12.536</v>
       </c>
-      <c r="I211" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J211" s="29">
+      <c r="I211" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J211" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -8962,10 +8962,10 @@
       <c r="H212" s="29">
         <v>12.536</v>
       </c>
-      <c r="I212" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J212" s="29">
+      <c r="I212" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J212" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -8994,10 +8994,10 @@
       <c r="H213" s="29">
         <v>12.536</v>
       </c>
-      <c r="I213" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J213" s="29">
+      <c r="I213" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J213" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -9026,10 +9026,10 @@
       <c r="H214" s="29">
         <v>12.536</v>
       </c>
-      <c r="I214" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J214" s="29">
+      <c r="I214" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J214" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -9058,10 +9058,10 @@
       <c r="H215" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I215" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J215" s="29">
+      <c r="I215" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J215" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -9090,10 +9090,10 @@
       <c r="H216" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I216" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J216" s="29">
+      <c r="I216" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J216" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -9122,10 +9122,10 @@
       <c r="H217" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I217" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J217" s="29">
+      <c r="I217" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J217" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -9154,10 +9154,10 @@
       <c r="H218" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I218" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J218" s="29">
+      <c r="I218" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J218" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -9186,10 +9186,10 @@
       <c r="H219" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I219" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J219" s="29">
+      <c r="I219" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J219" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -9218,10 +9218,10 @@
       <c r="H220" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I220" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J220" s="29">
+      <c r="I220" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J220" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -9250,10 +9250,10 @@
       <c r="H221" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I221" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J221" s="29">
+      <c r="I221" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J221" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -9282,10 +9282,10 @@
       <c r="H222" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I222" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J222" s="29">
+      <c r="I222" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J222" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -9314,10 +9314,10 @@
       <c r="H223" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I223" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J223" s="29">
+      <c r="I223" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J223" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -9346,10 +9346,10 @@
       <c r="H224" s="29">
         <v>1.1160000000000001</v>
       </c>
-      <c r="I224" s="29">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J224" s="29">
+      <c r="I224" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J224" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -9378,10 +9378,10 @@
       <c r="H225" s="29">
         <v>12.536</v>
       </c>
-      <c r="I225" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J225" s="29">
+      <c r="I225" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J225" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -9410,10 +9410,10 @@
       <c r="H226" s="29">
         <v>12.536</v>
       </c>
-      <c r="I226" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J226" s="29">
+      <c r="I226" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J226" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -9442,10 +9442,10 @@
       <c r="H227" s="29">
         <v>12.536</v>
       </c>
-      <c r="I227" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J227" s="29">
+      <c r="I227" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J227" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -9474,10 +9474,10 @@
       <c r="H228" s="29">
         <v>12.536</v>
       </c>
-      <c r="I228" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J228" s="29">
+      <c r="I228" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J228" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -9506,10 +9506,10 @@
       <c r="H229" s="29">
         <v>12.536</v>
       </c>
-      <c r="I229" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J229" s="29">
+      <c r="I229" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J229" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -9538,10 +9538,10 @@
       <c r="H230" s="29">
         <v>12.536</v>
       </c>
-      <c r="I230" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J230" s="29">
+      <c r="I230" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J230" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -9570,10 +9570,10 @@
       <c r="H231" s="29">
         <v>12.536</v>
       </c>
-      <c r="I231" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J231" s="29">
+      <c r="I231" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J231" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -9602,10 +9602,10 @@
       <c r="H232" s="29">
         <v>12.536</v>
       </c>
-      <c r="I232" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J232" s="29">
+      <c r="I232" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J232" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -9634,10 +9634,10 @@
       <c r="H233" s="29">
         <v>12.536</v>
       </c>
-      <c r="I233" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J233" s="29">
+      <c r="I233" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J233" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -9666,10 +9666,10 @@
       <c r="H234" s="29">
         <v>12.536</v>
       </c>
-      <c r="I234" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="J234" s="29">
+      <c r="I234" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J234" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>

</xml_diff>